<commit_message>
add names of teammate
</commit_message>
<xml_diff>
--- a/Security Task Team Information.xlsx
+++ b/Security Task Team Information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BFCAI\4th\Semester 7\opensource\Security-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D07611-060B-4F02-845B-507462F4CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D0288C-F1FE-4E9D-8E3E-45D865C666A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>لينك ال repo</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t>https://github.com/AbdallahHikal/Steganography.git</t>
+  </si>
+  <si>
+    <t>عبدالرحمن حسين أحمد</t>
+  </si>
+  <si>
+    <t>محمد الألفي محمد شريف</t>
+  </si>
+  <si>
+    <t>محمد بهاء محمد عطيه</t>
+  </si>
+  <si>
+    <t>أحمد غنيمي حلمي غنيمي</t>
+  </si>
+  <si>
+    <t>سعيد مجدي سعيد محمدي</t>
+  </si>
+  <si>
+    <t>حازم خالد منصور بيومي</t>
+  </si>
+  <si>
+    <t>https://github.com/Abdo3882/Open-source-pro</t>
   </si>
 </sst>
 </file>
@@ -135,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -145,6 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -364,23 +386,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="C9:F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="55.109375" customWidth="1"/>
+    <col min="2" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +426,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -425,11 +447,35 @@
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{03467FED-0208-4A25-A788-A9E8AD3C9445}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{81AB45AC-29BB-487B-A6A2-D5F77AA46D43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>